<commit_message>
Delete interpretable data in empty cells
</commit_message>
<xml_diff>
--- a/inputs/area_calib_empty.xlsx
+++ b/inputs/area_calib_empty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\218136\python_repo\Pond-IT\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\218136\python_repo\Pond-IT_1.3\Pond-IT\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E8BB64-1A3A-428D-A0FD-24D56B82637D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC18BC71-53FD-4B6B-9963-DD0090AF81AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="26610" windowHeight="16440" activeTab="1" xr2:uid="{59B4EB5B-337D-438F-9C32-8D149C92B367}"/>
+    <workbookView xWindow="4335" yWindow="0" windowWidth="12900" windowHeight="12000" xr2:uid="{59B4EB5B-337D-438F-9C32-8D149C92B367}"/>
   </bookViews>
   <sheets>
     <sheet name="Eagle" sheetId="2" r:id="rId1"/>
@@ -46,30 +46,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,24 +72,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,10 +394,10 @@
   <sheetPr codeName="Sheet25">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +405,7 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,211 +413,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="F2" s="1"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="5"/>
-      <c r="U2" s="5"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="F3" s="1"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="5"/>
-      <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="F4" s="1"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="5"/>
-      <c r="U4" s="5"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="F5" s="1"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="5"/>
-      <c r="U5" s="5"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="F6" s="1"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="5"/>
-      <c r="U6" s="5"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="F7" s="1"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="5"/>
-      <c r="U7" s="5"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="F8" s="1"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="5"/>
-      <c r="U8" s="5"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="F9" s="1"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="5"/>
-      <c r="U9" s="5"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="F10" s="1"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="5"/>
-      <c r="U10" s="5"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="F11" s="1"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="5"/>
-      <c r="U11" s="5"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="F12" s="1"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="5"/>
-      <c r="U12" s="5"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="F13" s="1"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="5"/>
-      <c r="U13" s="5"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="F14" s="1"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="5"/>
-      <c r="U14" s="5"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="F15" s="1"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="5"/>
-      <c r="U15" s="5"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="F16" s="1"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="5"/>
-      <c r="U16" s="5"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="F17" s="1"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="5"/>
-      <c r="U17" s="5"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="F18" s="1"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="5"/>
-      <c r="U18" s="5"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="F19" s="1"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="5"/>
-      <c r="U19" s="5"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="F20" s="1"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="5"/>
-      <c r="U20" s="5"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="F21" s="1"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="5"/>
-      <c r="U21" s="5"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="F22" s="1"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="5"/>
-      <c r="U22" s="5"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="Q23" s="2"/>
-      <c r="R23" s="5"/>
-      <c r="U23" s="5"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="Q24" s="2"/>
-      <c r="R24" s="5"/>
-      <c r="U24" s="5"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="Q25" s="2"/>
-      <c r="R25" s="5"/>
-      <c r="U25" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -655,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC90AB20-48D1-488A-938E-4C667DB2D1E5}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>